<commit_message>
Upload_Test_Files appear adaquate, CSV and XML parsers are hacked to work...
</commit_message>
<xml_diff>
--- a/Upload_Test_Files/test.xlsx
+++ b/Upload_Test_Files/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,28 +21,28 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
-    <t>temperature</t>
-  </si>
-  <si>
-    <t>capacity</t>
-  </si>
-  <si>
-    <t>color</t>
-  </si>
-  <si>
-    <t>comment</t>
-  </si>
-  <si>
-    <t>[Green,red,blue]</t>
-  </si>
-  <si>
-    <t>red</t>
-  </si>
-  <si>
-    <t>a comment</t>
-  </si>
-  <si>
-    <t>an other comment</t>
+    <t>sample1</t>
+  </si>
+  <si>
+    <t>comment 1</t>
+  </si>
+  <si>
+    <t>sample2</t>
+  </si>
+  <si>
+    <t>comment 2</t>
+  </si>
+  <si>
+    <t>sample3</t>
+  </si>
+  <si>
+    <t>comment 3</t>
+  </si>
+  <si>
+    <t>sample4</t>
+  </si>
+  <si>
+    <t>comment 4</t>
   </si>
 </sst>
 </file>
@@ -360,55 +360,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:D6"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>25.5</v>
+      </c>
+      <c r="C1">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>23.5</v>
+      </c>
+      <c r="C2">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+    </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B3">
-        <v>25</v>
+        <v>10.5</v>
       </c>
       <c r="C3">
-        <v>25</v>
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B4">
-        <v>100</v>
-      </c>
-      <c r="D4">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
+        <v>5.5</v>
+      </c>
+      <c r="C4">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="D4" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated parsers to define attributes as well as samples without hackyness, also updated CSV, XLS Test files.
</commit_message>
<xml_diff>
--- a/Upload_Test_Files/test.xlsx
+++ b/Upload_Test_Files/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="4650" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,30 +19,66 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>sample1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>comment 1</t>
   </si>
   <si>
-    <t>sample2</t>
-  </si>
-  <si>
     <t>comment 2</t>
   </si>
   <si>
-    <t>sample3</t>
-  </si>
-  <si>
     <t>comment 3</t>
   </si>
   <si>
-    <t>sample4</t>
-  </si>
-  <si>
     <t>comment 4</t>
+  </si>
+  <si>
+    <t># hash marks indicate file comments and are skipped.</t>
+  </si>
+  <si>
+    <t># '^' indicate attribute names.</t>
+  </si>
+  <si>
+    <t># Attribute types are parsed and determined to be floating-point, integer, arbitrary or [enumeration]</t>
+  </si>
+  <si>
+    <t>#Attribute Names:</t>
+  </si>
+  <si>
+    <t>^temperature</t>
+  </si>
+  <si>
+    <t>^capacity</t>
+  </si>
+  <si>
+    <t>^color</t>
+  </si>
+  <si>
+    <t>^comment</t>
+  </si>
+  <si>
+    <t>#Sample 1</t>
+  </si>
+  <si>
+    <t>[red]</t>
+  </si>
+  <si>
+    <t>#Sample 2</t>
+  </si>
+  <si>
+    <t>[green]</t>
+  </si>
+  <si>
+    <t>#Sample 3</t>
+  </si>
+  <si>
+    <t>[blue]</t>
+  </si>
+  <si>
+    <t>#Sample 4</t>
+  </si>
+  <si>
+    <t>[yellow]</t>
   </si>
 </sst>
 </file>
@@ -360,68 +396,112 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D4"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>25.5</v>
+      </c>
+      <c r="C6">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
-        <v>25.5</v>
-      </c>
-      <c r="C1">
-        <v>25</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>23.5</v>
+      </c>
+      <c r="C7">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>10.5</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>23.5</v>
-      </c>
-      <c r="C2">
-        <v>23</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9">
+        <v>5.5</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>10.5</v>
-      </c>
-      <c r="C3">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4">
-        <v>5.5</v>
-      </c>
-      <c r="C4">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
+      <c r="E9" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>